<commit_message>
Adding updated team schedule
</commit_message>
<xml_diff>
--- a/GA3331/Week8/GA3331 -Teams.xlsx
+++ b/GA3331/Week8/GA3331 -Teams.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="20115" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="20115" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="31">
   <si>
     <t>Monday</t>
   </si>
@@ -33,12 +33,6 @@
     <t>Friday</t>
   </si>
   <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
     <t>Team Name</t>
   </si>
   <si>
@@ -112,6 +106,9 @@
   </si>
   <si>
     <t>Asians in Paradise</t>
+  </si>
+  <si>
+    <t>11:00 AM - 1:00 PM</t>
   </si>
 </sst>
 </file>
@@ -127,12 +124,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -147,8 +162,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,18 +182,281 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1102345</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1245945</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9291</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="http://2.bp.blogspot.com/_eNOISzopUEs/S_rfLgkHe_I/AAAAAAAAAE8/-uZcOd5NWC4/s320/palm-tree.gif"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm flipH="1">
+          <a:off x="1102345" y="190499"/>
+          <a:ext cx="143600" cy="199792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3" descr="data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxQREhUSExQVFRQVGBsZGBgVFxQWGhoeFhccHRwdFxUcHCggGB0oHxUaJDIjJSkrLi4uGh8zODMsNystLisBCgoKDg0OGxAQGzckICQsLDAsLDQsLCwvLCwsLCwsNCwsLDQsLDQsLC0sLCwsLCwsLC4sLCwsLCw0LC4sLC8sLP/AABEIAJgAkAMBIgACEQEDEQH/xAAcAAACAwEBAQEAAAAAAAAAAAAABQQGBwMCAQj/xABDEAACAQICBQkECAQFBQEAAAABAgMAEQQhBRIxQVEGBxMiYXGBkaEyUrHBFDNTYnKCktEjQqLCJEOy8PEXNHOD4RX/xAAaAQACAwEBAAAAAAAAAAAAAAAAAwECBAUG/8QAKhEAAgIBBAEDAgcBAAAAAAAAAAECAxEEEiExQQUiURNxIzJhkaHh8BT/2gAMAwEAAhEDEQA/ANxooooAKKKKACiik+ltPLETHGvSzWvqKbBeBkfYg78+ANAJZHFFU/Daa0gM5IsK3YkkikdmsVINT4+UjD6zDSr2xlJR6EH0oyXdcl4LDRSTCcqsNJKsGuySvfVSRHjLW26usM/CndBQKKKKACiiigCpcrolxOJw2Fa5jUPNIASAdWyRhrHMEux/JSTmy5RFsRiMGxJTWeTDEsznUVyrKSbnLqkZ7G7KZ/SLvjMXttdE/Dh1Pxdm8qqXNXh/8cv3MO1/zMg+Rq+325E7/wARI2KiiiqDgooooAKj47GxwIZJXVEG1mIA/wCeyu7MALnIDaTVGkjGMxAxj3KICMMh2AHbKR7zWy4L30MvCDk8Im4nSs2Kyj1sPB7xFpnH3VP1S9p63YKMPhkjXVRQo295O0k7Se018xKOfYcKfvLrg9+YPkai9JiV9pIpBxR2Q/pYEetUbNkYKHRPr7elx0pq+3DOvaE6QeaXpHp/lTEV6LDyK8jX17XBjUe8DmCb2APbUPhDa475KK8iDTmO+kzNKCQMhGQbFQpuGU7iT1vKtF5B8rPpamCawxMYudwlXZrr8xuPeKy6vsbsrLJGxSRDdHG49o3g7CN4pUZ4fJ09VoI2VKMe10b/AEUh5IcpUx0RNgkyWEsd/ZJ2EcVO4/tT6tJ5mUXF4YVB05jxh8PLNt1EJA4m2QHebCp1VzlZLrvh8P779Iw+5BZv9ZQedBVvCyItLR/RdHMhN2WMKTxZvaPmTSjmlS+MxDblgjH6nc/2165zscVihiB+sZmPdGB83HlXXmYju+Mk/wDCnkHb+6myftMsFmxM1CiiilGsKKKh6W0guHiaVgTbIKNrMclVe0nKgBNypxJlYYNdjDWnI3JfJO9yCO4NXhRUbAwsoLOQZZDryEbNY7h90DIdgqRVGzdVDaj1S/SkkhMUUTBHlfV1iofVVVLMQpyJyAz41OqHhmDY0HdBCT+ad7D+mJvOgmx4iSRyfjA/iyTTH78hUfojCrbvBpTpXktBNHqIiwupujxqAQe33lO8GonOfywl0bBHJFGrvI5W7hiihRfMAi5N8s+NMeT2nOnwsWKkTojIusU25/d3kHdVmjKpNPKfJneLRoHaPEARuuZubKw95GO1fUb6gTaUX/LUv2nqr57T4Ux5d476TikDAWhQkDbYyn42QedJaQ4pM71OqtnWm/3LnzPwvLj5ZWb6qAAhRZf4rnVFtp+rY51stZ5zMYLVw8832sth3RDV+Ot51odOj0cLUS3WyYVUy/S4ueXaIwsC+HXkt4so/LVlxuKWKN5XNlRSxPYoufhVS0MDHh0L5O4Mj/ilOsR4a1vCmRWWZLZYRQucnEa2LCbo4lHi5JPwFWrmVitDin96YD9Ma/vWecocX02Kmk3FyB3J1flWocz0VsE7e9NIfKw+VWl0Lq/MXqiiilmkKqOOxP0mfWH1UBKpwaTYzdoX2R2luFMOWOknhhVISBPO4ijJ2KWBJb8qgnwFJMMzwoqHDsEUWBiIlFh2ZP6UNMZU4qXuYxAr4RUaLSUTGwkW/utdG/S1jXzEY0DZnS+jfFbujricSkal3YKqgkk7gNtVPkvyj18TL0q6n0llMJ4BFIWN+DWJYdpI3Uu5TaTM8nQg/wANDeTgzDYvcNp7bDjSPSWIVVttZvZANjcb7jMW23qu7nBrWiU6nKTx8f7+DWdIzxhLSqrg7FYBrnuNIsTiC5ubADYNgArO5tL4qSxkxMjEAC4CLs7lqJKuv7ZZvxMzehNqlzMMdHN9nXF4kSyySg3DudU/dXqi3gt/GuTvqgnhX0gKNwA8AKZ8lJxFP08uH6QJYwqzhRfO7OtibjKw3Z1Tt8m/DhDEVlo2jkLo84fAYeNhZhGCwPvNmb+Jp9VATl+zbThovxvIfgoqDjuX82fRSRP+CCS363kAPlTtyOR/y3N42vJZ+XuIHQJAT/3EioRxQdaT+lSPEVXNI6RPWcnJQT5C9U3SuksXi5EkmnYNEGCCNUUAPbWv1cz1RUHH4uZIpFd2kRxbXNgyXyOta2stt9sqZVbDoVq/TNUo78cLx5/YVwX1QTtOZ7zmfjW2808Wro6M+88jebmsW7Rsrc+bWLV0Zhe2PW/USfnUzMlHbZZqKKKoaCrafIkxsCfYRvKe9yET0169yTBdtL58RfE4qQbdZIh3RLc/1SHyriSTtpsY8GO2fuO2NdZRZ1VhwYA/Gqzp3DpCoEDPFK5smo51Rb2mKNdbAdm0in8jKilmNlUXJO4CqVpHSVmaeQEFskTeF/lUcCdp/wDlN2p9iPrThzF8ijEucKFRxra1wjD+c7Tr71O8nYfSlmbEsxux2n5AbhXvHu8us7ZvutsFswq9nxrnE97EbDnWO6CjL29HpdBrLL69try4nW1eWYAXJsBXzphewuzcFBY+mzxqVgMCzMHmW1j1Y7g5+85GRPAbqpCtyY7Va2rTx5eX8ELEQy6qygC2sLRsCTnsYi4zG5fnU+OPXAJdnB4dUeS5+dTsdmjW2gXHeM/lXApqN0i/VnNh7t/5h2cR48abbTx7Tn+neqbrNt/Un34X9HWPDquxQPD517rrXhhWNo9gljoErpXEGouksbqjVX2zv90ce/hUorOagssVY6RY5SiewQ1+CuATZeywzG6v0NyMw/R4DCpwhj9VB+dfnnC4SKSWCOVikTSqrsDYgOdU9Y7L62Z7TX6YwIQRqsRBRQFXVOsLKLAX37K1ReYnkdVBRucksZ5O9FFFSZzM9Bz9JAsu+YtLx+scsBfsBA8KZJTmbkfh7kw62HJ+yNlPfEbp6Uo0poTGRIxh6KdgDq/5bX3dU3VvNadGaMc6JZyhDyrxyxooZure7KNrEeyo8c/Cs+xuJLt0khA3AXyUcB8zvq6aG5usbiiJMW4gUeytxLLY7Sf5VY7Sc+GVduXHJXC4JMOsSFpHkJMjku1kQ8clF2GQAqzsT4RRUOKc5FEhDv7CEj3m6q+uZ8BT/kjyK6eOV5XLKjasai6KSM3vbNgCQoz3Go082opa17DIcTuA7zYVqWgcB9Gw8UP8yr1jxY5sfMmiSXGSKrJ84eM/BnzaPEZKBAltwFv+aHwfCr3pfRKyi4HWG+qjOpRirCxFOg4yRjsjKDFLxkZEV40OP4dvduv6TamMhvUXDJqvKvarfrH7qaMYZXdmOCFKnQsFH1bmy/dNr6vcQDbha3CvZNetIG8iL7oZj3nqr/dXKWUICzGwH+8uJrl6hJWNI9/6JbZPRxla/nD/AEXHJyxuIKL1UaRzfVRBctYXOXAbzUPD6Nlmu5KqDt1eufPYPWrHzdJ02PMpFjHC2V7212AHjkavWkeT0Mx17GOT7SPqk/iHsv4g02muOMyRyvVdfdKx11vCRlsOgEv1lMh++bj9Oz0pvo8TYc62HkeE/cPVPfGbqfKnmK5P4iNsgJV95MiPxIT8CfCl2uM7EGxsewjceFboxg0eZstuUsybyWTRXL2ZMsRD0gG14bBu8xMc/A+FW7RHKPDYr6qVS29DdHHejWI8qylplRdZiAO3/edINKSHEOgUkWdAluq2szgA620bdlKsqillGmjVTk8SXHyfoqiiis50QrLudLEXxcKfZwsT/wC11A9Iz51qNY/yzUyaQxBNuqI0HcFJ/vNXrXuEal4rYu5P4Pp8XChF1QmV+Fo7aoPexHlWn1k30eeN+lws7Qy6uqdhVwDcBgQd5OdS8DzgYiJzFiFRnFriwQ7NzLk1NmnkyVTjtwjTqXaX0Usy8GGw1Wf+oyDbh5Cd+q6el7VNg5e4Vxn0sZ4SJ80LCqptDJJSWGI8TAY21TkRUOWS0yH30ZT3qQy/Fqf4vSOGxPszRFt3WAPkar+lIygVtvRuGyzy2N6E09SyjBKvayE7XkkbtC+CD9yaS4jE9K1x7C+yOP3j8q+TYouoQbD1pDxLZ6o7M8/KvFcuTzJyPd1fh0QpXhLP38/yaDzT4fLEy8THGPygsfVxV+NVbm1h1cCrfaO7eF7D0WrSTWuHEUeb1Et1sn+oUh5T6IgeKSdgY3jRm6SPqt1QTZtzjsYGntVfnGxnR4MpvmdY/D2m9F9akTheTMVkd7NK2s9h2AZZhRuFN9CYTXxGGTe08Zyz9htc/wCmlKGtF5qNFdJLJi2HViHRx/ibOQ+A1R51aT4KVxzNJGpUUUUg3hVU5T8ikxTmeJzDOQATbWR7bOkTf3ixq10VKeOiJRUlhmO4zRWJwx/xEJA+0jvJH5gay/mA76ouNmSRpZDZkaQ2t1r6tlGrbedXK3Gv05SXEck8G8y4hsPH0qHWDBQMxsJAyYjiaZ9VtYZmWkjF5iZY3NnjEw6SqwkcjWeFsnW+wK5ycgbQbd9VaVSjFGVlddqsCGHeDX6WpPyg5M4fGraaMFh7Lr1XXucZ27NlUUmMlSn0fn8RhsiAe8Xr3Jo5GUrmtwRdSV29xq5aX5vMTh2JiH0iPcVssg7GQ5N3g+FVwoUfUcMje64KHyO3wpsWmZLFOIgw0eqoQixXI94/fbXt2sCeAJ8qnaWg1SJBsNlb+0/LyrnhNCvi1lCkrHGFDsOMjBUQdpuSeAHbWSdbUsHotPq4zo+o/Hf3Nj5MYbosHh04RLfvIufjTItaoE+PVequwZDuGVLcXpS2+tagzz0rUmPXxAFZxzjY/pZ4owcokLH8UhFvRPWnjaSLVQMbiellkk95jbuXqj4etWlDCKRt3NkYKxIVF1nYhUXizGwHma/RHJzRK4PDRYdf5FzPvMc2bxJJrLuarQ3T4pp2F0w4yvvkcZW/Ct/1CtjpM3ybaY4WQoooqg4KKKKACiiigAooooAKjY7ARTrqyxpIvB1DD1qTRQBSNMc2eGlVlieSDWBFgddc+Cts8DS3T+iY9G4PC4SM6xecM7sBrOY1LljbtVa0mqlzkcmXx2HBhYriICXisba1x1kJ4MB8KlPlZKSj7Wo8ZKZ9KJ31xmkvVZ//AEp4GEc6EP7ko6N+2x2P3jKmUWk4yLltTiGyt47K2RmmuDjTqnF8nbH4sxRO42hTbvOQ9TVYHUUAAmwAAG0nYAO0n4015QS3WNRmGbWJGYsg/cjyptzZ6G+k40MwvHhgJGuMixuIx6FvAUuyWDRpq8r7mq8jtC/QsJHCba9taQje7Zt+3hTuiisx1AooooAKKKKACiiigAooooAKKKKACiiigCNj8BFOhSaNJEO51DD12VRtNc1kL3bDSNCfdYGRPjrL4GiijJDSfZnGnuR+JwJMj4diFv14B0isDuIAuNxzFa/zbaDOEwa64tLMelk4gsMlPcthXyipbyVjBJ5Ra6KKKguf/9k="/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="1524000"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1714501</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>163785</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1965402</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>49019</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="http://cdn.bulbagarden.net/upload/thumb/6/6b/137Porygon.png/180px-137Porygon.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1714501" y="354285"/>
+          <a:ext cx="250901" cy="266234"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1064013</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>15054</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1555954</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>102219</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="http://techzwn.com/wp-content/uploads/2013/02/Global-Game-Jam-2013-620x350.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="31020" b="-31020"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1064013" y="586554"/>
+          <a:ext cx="491941" cy="277665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2680939</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>179820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3071231</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>18583</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="http://www.filmophilia.com/wp-content/uploads/2012/10/Live-Free-or-Die-Hard-Poster.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2680939" y="751320"/>
+          <a:ext cx="390292" cy="219763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:H2"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F16" totalsRowShown="0">
+  <autoFilter ref="A1:F16"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Monday"/>
     <tableColumn id="3" name="Tuesday"/>
     <tableColumn id="4" name="Wednesday"/>
     <tableColumn id="5" name="Thursday"/>
     <tableColumn id="6" name="Friday"/>
-    <tableColumn id="7" name="Saturday"/>
-    <tableColumn id="8" name="Sunday"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -481,25 +763,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -516,11 +794,306 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -535,103 +1108,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>